<commit_message>
camera aspect ratio updated
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -812,6 +812,40 @@
         </is>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2025-01-10 00:49:41</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2025-01-10 00:52:00</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
UI updated and file renamed
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -846,6 +846,108 @@
         </is>
       </c>
     </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2025-01-10 00:57:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2025-01-10 00:58:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2025-01-10 00:59:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2025-01-10 01:02:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>1446896_Asif Newaz</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2025-01-10 01:08:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>1446896_Asif Newaz</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2025-01-10 01:09:41</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Real time DB connected and cnn model added
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -948,6 +948,91 @@
         </is>
       </c>
     </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>1446896_Asif Newaz</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2025-01-10 11:20:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>1446896_Asif Newaz</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2025-01-12 12:08:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>1446896_Asif Newaz</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2025-01-12 12:09:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>1446896_Asif Newaz</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2025-01-12 12:10:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2025-01-12 12:12:17</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Database saving process added
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,6 +465,72 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Asif Newaz</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>2025-01-25</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>20:45:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Asif Newaz</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-01-25</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>23:02:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Asif Newaz</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2025-01-25</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>23:03:56</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Threshold added while detecting faces, and bug fixes for unknown model
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -531,6 +531,424 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Asif Newaz</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>14:46:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Asif Newaz</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>14:55:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Asif Newaz</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>14:56:55</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Asif Newaz</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>15:01:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Asif Newaz</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>15:07:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>1420867</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Mohsina Binte Asad</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>15:10:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Asif Newaz</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>15:10:48</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>1420867</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Mohsina Binte Asad</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>15:13:07</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>Asif Newaz</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>15:13:38</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>121212</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>Mukit</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>15:15:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>Asif Newaz</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>15:15:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>13131313</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Kamrul Hasan</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>15:18:21</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>13131313</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Kamrul Hasan</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>15:19:05</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>13131313</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Kamrul Hasan</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>15:20:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>13131313</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Kamrul Hasan</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>15:27:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>13131313</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Kamrul Hasan</t>
+        </is>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>15:29:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Asif Newaz</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>15:32:58</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>Asif Newaz</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>15:36:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>13131313</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>Kamrul Hasan</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>16:45:04</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
File path bug updated
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -949,6 +949,28 @@
         </is>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>1446896</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Asif Newaz</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2025-01-26</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>23:37:11</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Class Id added in sheet
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,20 +424,25 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>Class ID</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
           <t>ID</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Date</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>Time</t>
         </is>
@@ -446,44 +451,27 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>121212</t>
+          <t>12345</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Newaz</t>
+          <t>1446896</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-01-27</t>
+          <t>Asif Newaz</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>20:40:24</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>1446896</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Asif Newaz</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2025-01-27</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>21:02:50</t>
+          <t>2025-01-28</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>08:36:56</t>
         </is>
       </c>
     </row>

</xml_diff>